<commit_message>
VERSÃO Nº 1 - EXPLORANDO DADOS E CORRIGINDO ANOMARLIDADE NOS DADOS
</commit_message>
<xml_diff>
--- a/dados_1_cmt.xlsx
+++ b/dados_1_cmt.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\@IGOR\GIT\DESCOBRINDO ESTATÍSTICA COM R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Meu Drive\@IGOR\GIT\DESCOBRINDO ESTATISTICA COM R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{245E5F9D-6DBA-4C31-886A-D852F7241506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126F8208-5C17-4D96-BFAA-5B8A2676A3A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{397CB61E-C6FF-4DB6-82FD-DBBC4F70EE6E}"/>
+    <workbookView xWindow="-28920" yWindow="2925" windowWidth="29040" windowHeight="15840" xr2:uid="{397CB61E-C6FF-4DB6-82FD-DBBC4F70EE6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C72A60-E56F-4AEE-996D-02F5718312D5}">
-  <dimension ref="A1:B70"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,306 +415,306 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>13.5808</v>
+        <v>53.99505456</v>
       </c>
       <c r="B2" s="2">
-        <v>8.6791992187999991</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>6.5039999999999996</v>
+        <v>49.3536</v>
       </c>
       <c r="B3" s="2">
-        <v>4.5837402343999996</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>25.372800000000002</v>
+        <v>43.2776</v>
       </c>
       <c r="B4" s="2">
-        <v>13.61</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>17.616</v>
+        <v>42.783333320000004</v>
       </c>
       <c r="B5" s="2">
-        <v>13.623046875</v>
+        <v>10.66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>16.0928</v>
+        <v>41.526557359999998</v>
       </c>
       <c r="B6" s="2">
-        <v>11.63482666</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>14.7584</v>
+        <v>40.1584</v>
       </c>
       <c r="B7" s="2">
-        <v>11.463928223</v>
+        <v>17.744445801000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>10.220800000000001</v>
+        <v>40.041600000000003</v>
       </c>
       <c r="B8" s="2">
-        <v>5.0460815429999997</v>
+        <v>25.536804198999999</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>16.832000000000001</v>
+        <v>38.764800000000001</v>
       </c>
       <c r="B9" s="2">
-        <v>13.027954102000001</v>
+        <v>9.0225399999999993</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>13.0496</v>
+        <v>38.721600000000002</v>
       </c>
       <c r="B10" s="2">
-        <v>7.9956054688</v>
+        <v>19.579999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>14.646400000000002</v>
+        <v>38.302273016000001</v>
       </c>
       <c r="B11" s="2">
-        <v>5.5282592773000001</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>12.0832</v>
+        <v>36.419200000000004</v>
       </c>
       <c r="B12" s="2">
-        <v>5.5656433104999996</v>
+        <v>10.923461914059999</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>34.953600000000002</v>
+        <v>34.967967999999999</v>
       </c>
       <c r="B13" s="2">
-        <v>25.456115723</v>
+        <v>23.374511719000001</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>40.041600000000003</v>
+        <v>34.953600000000002</v>
       </c>
       <c r="B14" s="2">
-        <v>25.536804198999999</v>
+        <v>25.456115723</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>34.967967999999999</v>
+        <v>34.550167272000003</v>
       </c>
       <c r="B15" s="2">
-        <v>23.374511719000001</v>
+        <v>17.52</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>30.495999999999999</v>
+        <v>33.095784616000003</v>
       </c>
       <c r="B16" s="2">
-        <v>15.3</v>
+        <v>15.351013183599999</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>40.1584</v>
+        <v>31.944914284000003</v>
       </c>
       <c r="B17" s="2">
-        <v>17.744445801000001</v>
+        <v>17.518615723</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>15.84</v>
+        <v>30.495999999999999</v>
       </c>
       <c r="B18" s="2">
-        <v>9.7961425780999996</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>7.04</v>
+        <v>29.531199999999998</v>
       </c>
       <c r="B19" s="2">
-        <v>5.7922363281000004</v>
+        <v>10.663940429689999</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>15.3344</v>
+        <v>29.391999999999999</v>
       </c>
       <c r="B20" s="2">
-        <v>8.1863403320000003</v>
+        <v>8.9635478000000006</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>60.64</v>
+        <v>28.32</v>
       </c>
       <c r="B21" s="2">
-        <v>26.580810546999999</v>
+        <v>10.1974487305</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>19.910080000000001</v>
+        <v>26.716799999999999</v>
       </c>
       <c r="B22" s="2">
-        <v>12.334</v>
+        <v>13.438293457</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>16.464000000000002</v>
+        <v>26.504000000000001</v>
       </c>
       <c r="B23" s="2">
-        <v>12.635803223</v>
+        <v>9.0621948242200006</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>15.451079244000001</v>
+        <v>25.372800000000002</v>
       </c>
       <c r="B24" s="2">
-        <v>7.1304321288999999</v>
+        <v>13.61</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>14.912000000000001</v>
+        <v>24.622213591999998</v>
       </c>
       <c r="B25" s="2">
-        <v>9.423828125</v>
+        <v>17.52</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>18.206400000000002</v>
+        <v>24.473600000000001</v>
       </c>
       <c r="B26" s="2">
-        <v>10.516357422</v>
+        <v>8.4701538085900001</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>15.150208000000001</v>
+        <v>23.704000000000001</v>
       </c>
       <c r="B27" s="2">
-        <v>7.5103759765999998</v>
+        <v>12.802124022999999</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>11.888</v>
+        <v>22.9696</v>
       </c>
       <c r="B28" s="2">
-        <v>4.1885375976999999</v>
+        <v>4.8751831054999997</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>38.721600000000002</v>
+        <v>20.625599999999999</v>
       </c>
       <c r="B29" s="2">
-        <v>19.579999999999998</v>
+        <v>8.4426879882799994</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>12.65568</v>
+        <v>20.086400000000001</v>
       </c>
       <c r="B30" s="2">
-        <v>6.8725585938</v>
+        <v>4.5913696289099999</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>31.944914284000003</v>
+        <v>19.910080000000001</v>
       </c>
       <c r="B31" s="2">
-        <v>17.518615723</v>
+        <v>12.334</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>15.1472</v>
+        <v>19.261617020000003</v>
       </c>
       <c r="B32" s="2">
-        <v>4.6981811523000001</v>
+        <v>11.3651733398</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>23.704000000000001</v>
+        <v>19.090879999999999</v>
       </c>
       <c r="B33" s="2">
-        <v>12.802124022999999</v>
+        <v>12.539672852000001</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>49.3536</v>
+        <v>18.860800000000001</v>
       </c>
       <c r="B34" s="2">
-        <v>7.9696655273000001</v>
+        <v>8.0917358398000001</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>19.090879999999999</v>
+        <v>18.206400000000002</v>
       </c>
       <c r="B35" s="2">
-        <v>12.539672852000001</v>
+        <v>10.516357422</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>8.9024000000000001</v>
+        <v>17.705280000000002</v>
       </c>
       <c r="B36" s="2">
-        <v>3.6804199219</v>
+        <v>4.0481567382800003</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>18.860800000000001</v>
+        <v>17.616</v>
       </c>
       <c r="B37" s="2">
-        <v>8.0917358398000001</v>
+        <v>13.623046875</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>22.9696</v>
+        <v>16.832000000000001</v>
       </c>
       <c r="B38" s="2">
-        <v>4.8751831054999997</v>
+        <v>13.027954102000001</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>6.4</v>
+        <v>16.464000000000002</v>
       </c>
       <c r="B39" s="2">
-        <v>9.2526525999999993</v>
+        <v>12.635803223</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,245 +727,242 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>12.101120000000002</v>
+        <v>16.105360000000001</v>
       </c>
       <c r="B41" s="2">
-        <v>9.92138671875</v>
+        <v>10.1669311523</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>15.9808</v>
+        <v>16.0928</v>
       </c>
       <c r="B42" s="2">
-        <v>7.666015625</v>
+        <v>11.63482666</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>29.531199999999998</v>
+        <v>15.9808</v>
       </c>
       <c r="B43" s="2">
-        <v>10.663940429689999</v>
+        <v>7.666015625</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>14.6784</v>
+        <v>15.84</v>
       </c>
       <c r="B44" s="2">
-        <v>4.6112060546900002</v>
+        <v>9.7961425780999996</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>38.764800000000001</v>
+        <v>15.451079244000001</v>
       </c>
       <c r="B45" s="2">
-        <v>9.0225399999999993</v>
+        <v>7.1304321288999999</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>29.391999999999999</v>
+        <v>15.3344</v>
       </c>
       <c r="B46" s="2">
-        <v>8.9635478000000006</v>
+        <v>8.1863403320000003</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>36.419200000000004</v>
+        <v>15.150208000000001</v>
       </c>
       <c r="B47" s="2">
-        <v>10.923461914059999</v>
+        <v>7.5103759765999998</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
-        <v>24.473600000000001</v>
+        <v>15.1472</v>
       </c>
       <c r="B48" s="2">
-        <v>8.4701538085900001</v>
+        <v>4.6981811523000001</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>4.8032000000000004</v>
+        <v>14.912000000000001</v>
       </c>
       <c r="B49" s="2">
-        <v>3.0868530273399997</v>
+        <v>9.423828125</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>11.9552</v>
+        <v>14.7584</v>
       </c>
       <c r="B50" s="2">
-        <v>4.67529296875</v>
+        <v>11.463928223</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>13.524000000000001</v>
+        <v>14.6784</v>
       </c>
       <c r="B51" s="2">
-        <v>5.0704956054699997</v>
+        <v>4.6112060546900002</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>16.105360000000001</v>
+        <v>14.646400000000002</v>
       </c>
       <c r="B52" s="2">
-        <v>10.1669311523</v>
+        <v>5.5282592773000001</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>20.086400000000001</v>
+        <v>13.5808</v>
       </c>
       <c r="B53" s="2">
-        <v>4.5913696289099999</v>
+        <v>8.6791992187999991</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>20.625599999999999</v>
+        <v>13.524000000000001</v>
       </c>
       <c r="B54" s="2">
-        <v>8.4426879882799994</v>
+        <v>5.0704956054699997</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>12.486400000000001</v>
+        <v>13.0496</v>
       </c>
       <c r="B55" s="2">
-        <v>3.8116455078099998</v>
+        <v>7.9956054688</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>17.705280000000002</v>
+        <v>12.65568</v>
       </c>
       <c r="B56" s="2">
-        <v>4.0481567382800003</v>
+        <v>6.8725585938</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>26.504000000000001</v>
+        <v>12.486400000000001</v>
       </c>
       <c r="B57" s="2">
-        <v>9.0621948242200006</v>
+        <v>3.8116455078099998</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>10.614400000000002</v>
+        <v>12.101120000000002</v>
       </c>
       <c r="B58" s="2">
-        <v>5.2780151367199997</v>
+        <v>9.92138671875</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>28.32</v>
+        <v>12.0832</v>
       </c>
       <c r="B59" s="2">
-        <v>10.1974487305</v>
+        <v>5.5656433104999996</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>34.550167272000003</v>
+        <v>11.9552</v>
       </c>
       <c r="B60" s="2">
-        <v>17.52</v>
+        <v>4.67529296875</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>19.261617020000003</v>
+        <v>11.888</v>
       </c>
       <c r="B61" s="2">
-        <v>11.3651733398</v>
+        <v>4.1885375976999999</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>24.622213591999998</v>
+        <v>10.614400000000002</v>
       </c>
       <c r="B62" s="2">
-        <v>17.52</v>
+        <v>5.2780151367199997</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
-        <v>53.99505456</v>
+        <v>10.220800000000001</v>
       </c>
       <c r="B63" s="2">
-        <v>17.330200195300002</v>
+        <v>5.0460815429999997</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
-        <v>43.2776</v>
+        <v>9.7002666680000011</v>
       </c>
       <c r="B64" s="2">
-        <v>18</v>
+        <v>15.365</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
-        <v>38.302273016000001</v>
+        <v>8.9024000000000001</v>
       </c>
       <c r="B65" s="2">
-        <v>14</v>
+        <v>3.6804199219</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
-        <v>26.716799999999999</v>
+        <v>7.04</v>
       </c>
       <c r="B66" s="2">
-        <v>13.438293457</v>
+        <v>5.7922363281000004</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
-        <v>42.783333320000004</v>
+        <v>6.5039999999999996</v>
       </c>
       <c r="B67" s="2">
-        <v>10.66</v>
+        <v>4.5837402343999996</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
-        <v>41.526557359999998</v>
+        <v>6.4</v>
       </c>
       <c r="B68" s="2">
-        <v>14.3</v>
+        <v>9.2526525999999993</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <v>9.7002666680000011</v>
+        <v>4.8032000000000004</v>
       </c>
       <c r="B69" s="2">
-        <v>15.365</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
-        <v>33.095784616000003</v>
-      </c>
-      <c r="B70" s="2">
-        <v>15.351013183599999</v>
+        <v>3.0868530273399997</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{F7C72A60-E56F-4AEE-996D-02F5718312D5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B70">
+      <sortCondition descending="1" ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>